<commit_message>
Uploading data from fly emergence.
</commit_message>
<xml_diff>
--- a/data/fitness_experiment/fly_data.xlsx
+++ b/data/fitness_experiment/fly_data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_9/data/fitness_experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03ECA458-2C20-AD42-994B-C40CD0704847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C1AFE5-CE55-D848-B5DB-EC2377BB63CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{103D1930-54E4-A145-A095-23A50755D294}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{103D1930-54E4-A145-A095-23A50755D294}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,9 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F99C6F5-E500-6E49-A847-B1B0CE327204}">
   <dimension ref="A1:E1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1054" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G1073" sqref="G1073"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>